<commit_message>
updated based on new chatgpt.com ui and better practices
</commit_message>
<xml_diff>
--- a/test-file.xlsx
+++ b/test-file.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -402,13 +402,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="88.85546875" customWidth="1" min="1" max="1"/>
-    <col width="9.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="88.88671875" customWidth="1" min="1" max="1"/>
+    <col width="9.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="1">
@@ -431,8 +431,8 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sure! Here are the first 100 digits of the Fibonacci sequence:
-1, 1, 2, 3, 5, 8, 13, 21, 34, 55, 89, 144, 233, 377, 610, 987, 1597, 2584, 4181, 6765, 10946, 17711, 28657, 46368, 75025, 121393, 196418, 317811, 514229, 832040, 1346269, 2178309, 3524578, 5702887, 9227465, 14930352, 24157817, 39088169, 63245986, 102334155, 165580141, 267914296, 433494437, 701408733, 1134903170, 1836311903, 2971215073, 4807526976, 7778742049, 12586269025, 20365011074, 32951280099, 53316291173, 86267571272, 139583862445, 225851433717, 365435296162, 591286729879, 956722026041, 1548008755920, 2504730781961, 4052739537881, 6557470319842, 10610209857723, 17167680177565, 27777890035288, 44945570212853, 72723460248141, 117669030460994, 190392490709135, 308061521170129, 498454011879264, 806515533049393, 1304969544928657, 2111485077978050, 3416454622906707, 5527939700884757, 8944394323791464, 14472334024676221, 23416728348467685, 37889062373143906, 61305790721611591, 99194853094755497, 160500643816367088, 259695496911122585, 420196140727489673, 679891637638612258</t>
+          <t>Here are the first 100 digits of the Fibonacci sequence:
+1, 1, 2, 3, 5, 8, 13, 21, 34, 55, 89, 144, 233, 377, 610, 987, 1597, 2584, 4181, 6765, 10946, 17711, 28657, 46368, 75025, 121393, 196418, 317811, 514229, 832040, 1346269, 2178309, 3524578, 5702887, 9227465, 14930352, 24157817, 39088169, 63245986, 102334155, 165580141, 267914296, 433494437, 701408733, 1134903170, 1836311903, 2971215073, 4807526976, 7778742049, 12586269025, 20365011074, 32951280099, 53316291173, 86267571272, 139583862445, 225851433717, 365435296162, 591286729879, 956722026041, 1548008755920, 2504730781961, 4052739537881, 6557470319842, 10610209857723, 17167680177565, 27777890035288, 44945570212853, 72723460248141, 117669030460994, 190392490709135, 308061521170129, 498454011879264, 806515533049393, 1304969544928657, 2111485077978050, 3416454622906707, 5527939700884757, 8944394323791464, 14472334024676221, 23416728348467685, 37889062373143906, 61305790721611591, 99194853094755497, 160500643816367088, 259695496911122585, 420196140727489673, 679891637638612258, 1100087778366101931, 1779979416004714189, 2880067194370816120, 4660046610375530309, 7540113804746346429, 12200160415121876738, 19740274219868223167, 31940434634990099905, 51680708854858323072, 83621143489848422977, 135301852344706746049, 218922995834555169026.</t>
         </is>
       </c>
     </row>
@@ -444,8 +444,8 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sure! Here are the first 100 digits of Pi (π):
-3.1415926535 8979323846 2643383279 5028841971 6939937510 5820974944 5923078164 0628620899 8628034825 3421170679 8214808651 3282306647 0938446095 5058223172 5359408128 4811174502 8410270193 8521105559 6446229489 5493038196 4428810975 6659334461 2847564823 3786783165 2712019091 4564856692 3460348610 4543266482 1339360726 0249141273 7245870066 0631558817 4881520920 9628292540 9171536436 7892590360 0113305305 4882046652 1384146951 9415116094 3305727036 0011330530 5465237338 9053332563 8218182845 3566370084 7350152114 8170866229 4077247203 4532301953 4301465495 9455346908 4282340288 4197169399 3751058209 7494459230 5305488204 6652139282 3066470938 4460955058 2231725359 4081284811 1745028410 2701938521 3841469519 9766932027 7053921717 6265470136 5534068213 9494634284 7564823378 6783165271 4526356082 7785771342 7577896091 7363717872 1468440901 2249534301 4654958537 1050792279 6892589235 4201995611 2129021960 8640344181 5981362977 4771309960 5187072113 4999999837 2978049951 0597317328 1609631859 5024459455 3469083026 4252230825 3344685035 2619311881 7101000313 7838752886 5875332083 8142061717 7669147303 5982534904 2875546873 1159562863 8823537875 9375195778 1857780532 1712268066 1300192787 6611195909 2164201989 4676783744 9448255379 7747268471 0359825344 6850352619 5965593644 6229489549 3038196477 8662599403 6785473518 8615024459 2305811859 5024459455 3469083026 4252230825 3344685035 2619311881 7101000313 7838752886 5875332083 8142061717 7669147303 5982534904 2875546873 1159562863 8823537875 9375195778 1857780532 1712268066 1300192787 6611195909 2164201989 4676783744 9448255379 7747268471 0359825344 6850352619 5965593644 6229489549 3038196477 8662599403 6785473518 8615024459 2305811859</t>
+          <t>Here are the first 100 digits of Pi (π):
+3.1415926535 8979323846 2643383279 5028841971 6939937510 5820974944 5923078164 0628620899 8628034825 3421170679</t>
         </is>
       </c>
     </row>
@@ -457,8 +457,8 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Certainly! Here are the first 100 digits of Euler's number (e):
-2.7182818284 5904504710 9950113305 8223172535 9408128481 1174502841 0270193852 1105559644 6229489549 3038196442 8810975665 9334461284 7564823378 6783165271 4526356082 7785771342 7577896091 7363717872 1468440901 2249534301 4654958537 1050792279 6892589235 4201995611 2129021960 8640344181 5981362977 4771309960 5187072113 4999999837 2978049951 0597317328 1609631859 5024459455 3469083026 4252230825 3344685035 2619311881 7101000313 7838752886 5875332083 8142061717 7669147303 5982534904 2875546873 1159562863 8823537875 9375195778 1857780532 1712268066 1300192787 6611195909 2164201989 4676783744 9448255379 7747268471 0359825344 6850352619 5965593644 6229489549 3038196477 8662599403 6785473518 8615024459 2305811859 5024459455</t>
+          <t>Here are the first 100 digits of Euler's number (e):
+2.7182818284 5904523536 0287471352 6624977572 4709369995 9574966967 6277240766 3035354759 4571382178 5251664274</t>
         </is>
       </c>
     </row>
@@ -470,31 +470,31 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sure! Here’s a fun and adventurous story for an 11-year-old:
-The Secret of the Whispering Woods
-Once upon a time, in the small town of Willowbrook, there was a mysterious forest known as the Whispering Woods. The trees in this forest were ancient and tall, their branches entwined like old friends. The townsfolk whispered that the woods were magical and that they held secrets beyond imagination.
-One sunny afternoon, 11-year-old Emma and her best friend Max decided to explore the Whispering Woods. Emma was known for her curiosity, always asking questions and seeking answers. Max, on the other hand, was brave and loved adventure. Together, they made the perfect team.
-“Are you sure we should do this?” Max asked, his eyes wide with excitement and a bit of fear.
-“Absolutely!” Emma replied, holding up a map she had drawn based on old stories and legends about the forest. “We’ve got to find out what’s making the trees whisper.”
-As they entered the forest, the air was filled with the sound of rustling leaves. Emma and Max followed a narrow path that seemed to be leading them deeper into the woods. They marveled at the enormous trees, their bark covered in moss and their leaves shimmering in the sunlight.
-After a while, they came across a small, sparkling stream. Emma noticed something peculiar: the water seemed to glow with a soft, blue light. “Look at this!” she said, pointing to the stream.
-Max knelt by the water and dipped his fingers in. “It feels warm and tingly. Do you think this is magic?”
-Before Emma could answer, they heard a soft, melodious voice coming from the trees. “Welcome, travelers,” it said.
-Emma and Max looked around, trying to find the source of the voice. Suddenly, a small, shimmering creature appeared on a nearby branch. It was no bigger than a squirrel but had delicate, iridescent wings and a glowing aura.
-“I am Lumina, the guardian of the Whispering Woods,” the creature said with a gentle smile. “I’ve been waiting for brave souls like you.”
-“What’s the secret of the Whispering Woods?” Emma asked eagerly.
-Lumina fluttered her wings and hovered above them. “The forest is alive with magic, but it needs your help. An ancient spell has been cast, causing the trees to whisper in sorrow. The spell can only be broken by finding three magical crystals hidden in the woods.”
-Max’s eyes lit up. “That sounds like an adventure! How do we find the crystals?”
-Lumina pointed to the stream. “The first crystal lies beneath the surface of this stream. It will reveal itself to those who are pure of heart.”
-Emma and Max carefully waded into the stream, feeling the warm, glowing water swirl around their feet. They searched for a while until Emma’s hand brushed against something smooth and cool. She reached down and pulled out a small, blue crystal that sparkled like a star.
-“That’s one!” Lumina exclaimed. “Now, you must find the second crystal, which is hidden in the Heart of the Forest. Follow the path of the glowing fireflies to guide your way.”
-As they continued their journey, tiny fireflies began to appear, lighting up the path with their soft, golden glow. Emma and Max followed the fireflies until they reached a magnificent oak tree at the heart of the forest. The second crystal was nestled in a hollow of the tree, surrounded by glowing flowers.
-With two crystals in hand, they made their way to the final destination: a hidden cave covered in ivy. The entrance was dark and mysterious, but Emma and Max bravely stepped inside. The cave was filled with glittering crystals and ancient carvings. In the center of the cave was a pedestal holding the third crystal, which glowed with a bright, green light.
-As they placed the third crystal on the pedestal, the entire cave illuminated with a dazzling light. The spell was broken, and the forest seemed to come alive with joy. The trees stopped whispering in sorrow and began to sing a cheerful melody.
-Lumina appeared once more, her wings sparkling with happiness. “You have done it! The Whispering Woods are free from the spell, and its magic will now thrive. Thank you for your bravery and kindness.”
-Emma and Max were overjoyed with their adventure. They bid farewell to Lumina and made their way back to Willowbrook, their hearts full of wonder and excitement.
-From that day on, the Whispering Woods became a place of joy and magic, visited by many who wanted to experience its wonder. Emma and Max’s adventure was told and retold, becoming a beloved legend in Willowbrook. And every time they walked through the woods, they remembered the day they helped save the magical forest and the friend they had made along the way.
-I hope you enjoyed the story!</t>
+          <t>The Quest for the Lost Dragon Egg
+In a small village nestled between rolling hills and enchanted forests, there lived an 11-year-old boy named Leo. Leo was curious, adventurous, and always dreamed of becoming a great explorer like the heroes in the stories his grandfather told him. He had a best friend named Lily, who was just as daring as he was, and together they were always getting into some kind of mischief.
+One crisp autumn morning, Leo and Lily decided to venture into the Whispering Woods, a place no one in the village dared to go. The woods were known for their towering trees that seemed to whisper secrets when the wind blew, and for the strange creatures said to live deep within. But Leo and Lily were not afraid—well, maybe just a little—but that was what made the adventure exciting.
+As they entered the forest, the air felt different. The whispers of the trees sounded like soft voices, as if they were calling out to them. The path beneath their feet was covered in golden leaves, and the sunlight barely made it through the thick canopy above.
+“We should turn back,” Lily whispered, though she didn’t really mean it.
+Leo grinned. “Are you kidding? This is just getting good!”
+After walking for what felt like hours, they came upon an old stone bridge crossing a shimmering river. As they approached, they saw something strange—a small creature sitting on the edge of the bridge. It had the body of a lizard, wings like a bat, and the tiniest puff of smoke curled from its nose.
+“A dragon!” Leo gasped.
+The creature was barely the size of a cat, but it was unmistakably a baby dragon. Its scales gleamed in the sunlight, shifting colors from blue to green to gold.
+The dragon blinked at them, looking as surprised as they were. It let out a tiny roar, which sounded more like a squeaky toy, and then quickly flapped its wings and darted off into the woods.
+“Wait!” Leo shouted, chasing after it. Lily followed, her heart pounding with excitement.
+They ran deeper into the forest, following the flashes of color from the dragon’s scales, until they reached a clearing. In the center of the clearing was something they had only heard about in legends: a massive dragon’s nest. It was made of branches, leaves, and shimmering stones, but what caught their attention most was the large, glowing egg sitting in the middle of it.
+“This is it!” Leo whispered in awe. “The lost dragon egg!”
+According to the legends, the dragons had left the village long ago after a terrible storm destroyed their home. The villagers believed that one day, a brave soul would find the last dragon egg and bring peace between humans and dragons once more. But no one had seen a dragon in years—until now.
+Before they could get any closer, the ground shook. The trees trembled, and a shadow fell over the clearing. From above, a giant dragon swooped down, landing with a thud in front of the nest. Its eyes were fierce, but there was something gentle about the way it glanced at the egg.
+Leo and Lily froze. They had never been so close to such a powerful creature.
+The dragon let out a low growl, but instead of attacking, it stepped back, watching them closely.
+“I think it’s...waiting,” Lily whispered. “Maybe it wants us to do something.”
+Leo’s heart raced. What were they supposed to do? Then, he remembered something his grandfather had told him about dragons: “They only trust those who are brave but kind.”
+He took a deep breath, slowly walked forward, and knelt beside the egg. “We’re not here to hurt you,” he said softly. “We just want to help.”
+The dragon tilted its head, watching him closely.
+Lily, feeling a little braver now, stepped up beside Leo. “We’ll protect your egg,” she said. “We promise.”
+Suddenly, the egg began to glow brighter, and tiny cracks appeared on its surface. The dragon’s eyes widened, and it let out a soft rumble of approval.
+The egg was hatching!
+Leo and Lily watched in amazement as the shell broke apart, and a tiny dragon emerged. It was no bigger than a rabbit, with shimmering silver scales and bright blue eyes. It looked up at them, blinking in the sunlight, and let out a</t>
         </is>
       </c>
     </row>
@@ -504,23 +504,7 @@
           <t>How is cheese made</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Cheese-making is a fascinating process that transforms milk into a wide variety of delicious cheeses. Here’s a basic overview of how cheese is made:
-Milk Collection: Cheese starts with milk, usually from cows, goats, or sheep. The quality of the milk is crucial, so it's often fresh and high-quality.
-Pasteurization (Optional): Some cheeses are made with pasteurized milk, which means the milk is heated to kill any harmful bacteria. Others use raw milk, which has not been pasteurized.
-Acidification: Bacteria are added to the milk to begin the acidification process. These bacteria ferment the lactose (milk sugar) into lactic acid, which helps to coagulate the milk and gives the cheese its flavor.
-Coagulation: An enzyme called rennet (or sometimes an alternative coagulant) is added to the milk. Rennet causes the milk proteins (casein) to form curds and separates them from the whey (the liquid part). This forms a gel-like substance.
-Cutting the Curd: The curds are cut into small pieces to help release the whey. The size of the curds can affect the texture of the cheese. For some cheeses, the curds are cut very small, while for others, they might be larger.
-Cooking and Stirring: The curds are gently heated and stirred to help them release more whey and firm up. The temperature and duration of this step can vary depending on the type of cheese being made.
-Draining the Whey: The whey is drained from the curds. This can be done by pouring the mixture into a cheesecloth-lined mold or using special equipment.
-Pressing: The curds are placed into molds and pressed to remove any remaining whey and to shape the cheese. The amount of pressure and the duration can influence the texture of the final cheese.
-Salting: After pressing, the cheese is salted. Salt enhances flavor, helps in preserving the cheese, and aids in the formation of the rind. Salt can be added directly to the curds or applied to the surface of the cheese.
-Aging (Maturation): Many cheeses are aged in a controlled environment to develop their flavor and texture. Aging can range from a few weeks to several years, depending on the type of cheese. During aging, cheeses may be turned, washed, or treated with special bacteria or molds.
-Finishing Touches: Some cheeses undergo additional processes, like coating with wax, rubbing with herbs or spices, or adding flavorings. This can affect the texture and flavor of the cheese.
-Each cheese variety has its own unique steps and techniques, which contribute to its distinct taste and texture. From creamy Brie to sharp Cheddar, the art of cheese-making offers endless possibilities!</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>